<commit_message>
Update: Atualizando a documentação
</commit_message>
<xml_diff>
--- a/doc/projeto.xlsx
+++ b/doc/projeto.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camila.yjodai\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.hsantos43\Documents\esquinadesampa\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9541C1D5-E28D-49F7-8007-A56B6465509B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B70FAC-044B-4699-B868-69F29E5AD8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0A39003E-D5B8-4D6E-90E9-0089D8B2E310}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
   <si>
     <t>RESTAURANTE</t>
   </si>
@@ -173,38 +172,131 @@
     <t>2 NORMALIZAÇÃO</t>
   </si>
   <si>
-    <t>idrestaurante 1:1</t>
-  </si>
-  <si>
-    <t>idcontato 1:1</t>
-  </si>
-  <si>
-    <t>idendereco 1:1</t>
-  </si>
-  <si>
-    <t>idfoto 1:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idlogin 1:1 </t>
-  </si>
-  <si>
-    <t>idfeedback 1:1</t>
-  </si>
-  <si>
-    <t>idrestaurante 1:n</t>
-  </si>
-  <si>
-    <t>idfeedback 1:n</t>
-  </si>
-  <si>
-    <t>idfoto 1:n</t>
+    <t>idrestaurante 1:1 INT AUT_INCRE</t>
+  </si>
+  <si>
+    <t>idcontato 1:1 INT AUT_INC</t>
+  </si>
+  <si>
+    <t>idendereco 1:1 INT AUT_INC</t>
+  </si>
+  <si>
+    <t>idfoto 1:1 INT AUT_INC</t>
+  </si>
+  <si>
+    <t>idlogin 1:1  INT AUT_INC</t>
+  </si>
+  <si>
+    <t>idfeedback 1:1 INT AUT_INC</t>
+  </si>
+  <si>
+    <t>idcontato 1:1 INT</t>
+  </si>
+  <si>
+    <t>idendereco 1:1INT</t>
+  </si>
+  <si>
+    <t>nomerestaurante VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>cnpj VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>faixadepreco INT</t>
+  </si>
+  <si>
+    <t>descricao TEXT</t>
+  </si>
+  <si>
+    <t>idfeedback 1:n INT</t>
+  </si>
+  <si>
+    <t>idfoto 1:n INT</t>
+  </si>
+  <si>
+    <t>datacriacao DAT E</t>
+  </si>
+  <si>
+    <t>status VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>telefoneresidencial VARCHAR(15)</t>
+  </si>
+  <si>
+    <t>email VARCHA(100)</t>
+  </si>
+  <si>
+    <t>telefonecelular VARCHAR(15)</t>
+  </si>
+  <si>
+    <t>site VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>categoria ENUM</t>
+  </si>
+  <si>
+    <t>horariofuncionamento DATETIME</t>
+  </si>
+  <si>
+    <t>logradouro VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>numero VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>complemento VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>bairro VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>cep VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>estado VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>cidade VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>fotocapa TEXT</t>
+  </si>
+  <si>
+    <t>foto1 TEXT</t>
+  </si>
+  <si>
+    <t>foto2 TEXT</t>
+  </si>
+  <si>
+    <t>usuario VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>email VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>senhaVARCHAR(100)</t>
+  </si>
+  <si>
+    <t>datacadastro DATE</t>
+  </si>
+  <si>
+    <t>idrestaurante 1:n INT</t>
+  </si>
+  <si>
+    <t>nome VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>opiniao VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>nota INT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,22 +811,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A890F1AA-3556-47D9-A8D9-9C3C6B0E13BF}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -754,7 +846,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -774,7 +866,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -794,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -814,7 +906,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -834,7 +926,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -852,7 +944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -866,7 +958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -878,7 +970,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -890,7 +982,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -900,7 +992,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -910,7 +1002,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -920,7 +1012,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="15" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1032,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="12" t="s">
         <v>1</v>
       </c>
@@ -963,7 +1055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -986,7 +1078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1009,7 +1101,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1029,7 +1121,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="13" t="s">
         <v>3</v>
       </c>
@@ -1047,7 +1139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
@@ -1061,7 +1153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1073,7 +1165,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1177,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="13" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1187,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1105,7 +1197,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="13" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1207,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1125,7 +1217,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -1135,7 +1227,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="16" t="s">
         <v>44</v>
       </c>
@@ -1145,7 +1237,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="15" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="12" t="s">
         <v>45</v>
       </c>
@@ -1185,125 +1277,125 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="B36" s="14" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="13" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="14" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="13" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1311,9 +1403,9 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1321,9 +1413,9 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="13" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1331,9 +1423,9 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1341,9 +1433,9 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>

</xml_diff>

<commit_message>
Update: Atualização da Doc
</commit_message>
<xml_diff>
--- a/doc/projeto.xlsx
+++ b/doc/projeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.hsantos43\Documents\esquinadesampa\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B70FAC-044B-4699-B868-69F29E5AD8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA512BA-F87F-452D-896F-AE171ACF4F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0A39003E-D5B8-4D6E-90E9-0089D8B2E310}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
   <si>
     <t>RESTAURANTE</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>descricao TEXT</t>
-  </si>
-  <si>
-    <t>idfeedback 1:n INT</t>
   </si>
   <si>
     <t>idfoto 1:n INT</t>
@@ -296,8 +293,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -451,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -475,6 +480,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,24 +815,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A890F1AA-3556-47D9-A8D9-9C3C6B0E13BF}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -846,7 +852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -866,7 +872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -886,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -906,7 +912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -926,7 +932,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -944,7 +950,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -958,7 +964,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -970,7 +976,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -982,7 +988,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -992,7 +998,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1002,7 +1008,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -1012,7 +1018,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>3</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1165,7 +1171,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1177,7 +1183,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1193,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1197,7 +1203,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1213,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1217,7 +1223,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -1227,7 +1233,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>44</v>
       </c>
@@ -1237,7 +1243,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>45</v>
       </c>
@@ -1277,125 +1283,125 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F35" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="13" t="s">
-        <v>57</v>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1403,9 +1409,9 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1" t="s">
-        <v>59</v>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1413,9 +1419,9 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="13" t="s">
-        <v>58</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1423,9 +1429,9 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="1" t="s">
-        <v>66</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1433,17 +1439,19 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="2" t="s">
-        <v>60</v>
-      </c>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>